<commit_message>
Added scenarios for Login, inbox, unread, Forgot password
</commit_message>
<xml_diff>
--- a/TestData/AnswerConnectData.xlsx
+++ b/TestData/AnswerConnectData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Valid Email ID</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Invalid Password</t>
   </si>
   <si>
+    <t>Invalid Email format</t>
+  </si>
+  <si>
     <t>answerconnectand@gmail.com</t>
   </si>
   <si>
@@ -39,16 +42,19 @@
   <si>
     <t>test13</t>
   </si>
+  <si>
+    <t>answerconnectand</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -70,6 +76,103 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -83,16 +186,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -101,72 +197,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,31 +211,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,49 +232,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,13 +376,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,115 +406,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,8 +444,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -455,6 +461,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -476,9 +491,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,19 +503,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,160 +538,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1010,21 +1016,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="31.453125" customWidth="1"/>
     <col min="2" max="2" width="20.546875" customWidth="1"/>
     <col min="3" max="3" width="26.171875" customWidth="1"/>
     <col min="4" max="4" width="27.8671875" customWidth="1"/>
+    <col min="5" max="5" width="29.4296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1037,25 +1044,32 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" ht="28" customHeight="1" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="2" ht="28" customHeight="1" spans="1:5">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="answerconnectand@gmail.com" tooltip="mailto:answerconnectand@gmail.com"/>
     <hyperlink ref="C2" r:id="rId2" display="testmail@gmail.com" tooltip="mailto:testmail@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="answerconnectand" tooltip="mailto:answerconnectand@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>